<commit_message>
lab 2a eixos do grafico
</commit_message>
<xml_diff>
--- a/lab2a/tabelas/tabelas comando conversor.xlsx
+++ b/lab2a/tabelas/tabelas comando conversor.xlsx
@@ -584,16 +584,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="216276360"/>
-        <c:axId val="216138472"/>
+        <c:axId val="236533760"/>
+        <c:axId val="236646384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="216276360"/>
+        <c:axId val="236533760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ângulo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de disparo [º]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -631,7 +692,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216138472"/>
+        <c:crossAx val="236646384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -639,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216138472"/>
+        <c:axId val="236646384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,6 +720,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Tensão na carga [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -690,7 +807,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216276360"/>
+        <c:crossAx val="236533760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1651,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added tables for 5.2 question
</commit_message>
<xml_diff>
--- a/lab2a/tabelas/tabelas comando conversor.xlsx
+++ b/lab2a/tabelas/tabelas comando conversor.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5.2.f" sheetId="1" r:id="rId1"/>
+    <sheet name="5.2.j" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Vo teórico [V]</t>
   </si>
@@ -24,6 +28,36 @@
   <si>
     <t xml:space="preserve"> Ângulo de Disparo - α [º]</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Ângulo de Condução - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>γ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> [º]</t>
+    </r>
+  </si>
+  <si>
+    <t>Io teórico [mA]</t>
+  </si>
+  <si>
+    <t>Io experimental [mA]</t>
+  </si>
 </sst>
 </file>
 
@@ -32,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +81,12 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -56,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -266,11 +306,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -305,12 +436,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -325,7 +505,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -401,7 +581,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -584,11 +764,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="216276360"/>
-        <c:axId val="216138472"/>
+        <c:axId val="402026632"/>
+        <c:axId val="402028984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="216276360"/>
+        <c:axId val="402026632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,10 +808,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216138472"/>
+        <c:crossAx val="402028984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -639,7 +819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216138472"/>
+        <c:axId val="402028984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,10 +867,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216276360"/>
+        <c:crossAx val="402026632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,7 +910,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -760,7 +940,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1363,7 +1543,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1651,19 +1831,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="22.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="22.7265625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1680,7 +1860,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -1703,7 +1883,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C4" s="4"/>
       <c r="D4" s="9">
         <v>0</v>
@@ -1727,7 +1907,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C5" s="4"/>
       <c r="D5" s="9">
         <v>30</v>
@@ -1751,7 +1931,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C6" s="4"/>
       <c r="D6" s="9">
         <v>60</v>
@@ -1775,7 +1955,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C7" s="4"/>
       <c r="D7" s="9">
         <v>90</v>
@@ -1799,7 +1979,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C8" s="4"/>
       <c r="D8" s="9">
         <v>120</v>
@@ -1823,7 +2003,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="4"/>
       <c r="D9" s="12">
         <v>150</v>
@@ -1847,7 +2027,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1864,7 +2044,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1881,7 +2061,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1898,7 +2078,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1915,7 +2095,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1932,7 +2112,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1949,7 +2129,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1966,7 +2146,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1983,7 +2163,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2000,7 +2180,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2017,7 +2197,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2034,7 +2214,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2056,4 +2236,379 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:T17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25" style="3" customWidth="1"/>
+    <col min="6" max="9" width="22.7265625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C3" s="4"/>
+      <c r="D3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C4" s="4"/>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16">
+        <v>30.4</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="19">
+        <v>170</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="4"/>
+      <c r="D5" s="12">
+        <v>90</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17">
+        <v>15.2</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="20">
+        <v>88</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+      <c r="D9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="1"/>
+      <c r="D11" s="12">
+        <v>90</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added tables 5.2i and 5.2j
</commit_message>
<xml_diff>
--- a/lab2a/tabelas/tabelas comando conversor.xlsx
+++ b/lab2a/tabelas/tabelas comando conversor.xlsx
@@ -4,17 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5.2.f" sheetId="1" r:id="rId1"/>
+    <sheet name="5.2.j" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Vo teórico [V]</t>
   </si>
@@ -24,6 +29,36 @@
   <si>
     <t xml:space="preserve"> Ângulo de Disparo - α [º]</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Ângulo de Condução - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>γ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> [º]</t>
+    </r>
+  </si>
+  <si>
+    <t>Io experimental [mA]</t>
+  </si>
+  <si>
+    <t>Io teórico [mA]</t>
+  </si>
 </sst>
 </file>
 
@@ -32,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +82,12 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -56,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -266,11 +307,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -305,12 +437,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -325,7 +506,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -375,7 +556,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -401,7 +581,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -584,11 +764,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="236533760"/>
-        <c:axId val="236646384"/>
+        <c:axId val="249641184"/>
+        <c:axId val="249642752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236533760"/>
+        <c:axId val="249641184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +805,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -651,7 +830,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -689,10 +868,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236646384"/>
+        <c:crossAx val="249642752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -700,7 +879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236646384"/>
+        <c:axId val="249642752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +925,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -772,7 +950,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -804,10 +982,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236533760"/>
+        <c:crossAx val="249641184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -821,7 +999,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -847,7 +1024,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -877,7 +1054,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1480,7 +1657,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1768,19 +1945,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="22.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="22.7265625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1797,7 +1974,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -1820,7 +1997,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C4" s="4"/>
       <c r="D4" s="9">
         <v>0</v>
@@ -1844,7 +2021,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C5" s="4"/>
       <c r="D5" s="9">
         <v>30</v>
@@ -1868,7 +2045,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C6" s="4"/>
       <c r="D6" s="9">
         <v>60</v>
@@ -1892,7 +2069,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C7" s="4"/>
       <c r="D7" s="9">
         <v>90</v>
@@ -1916,7 +2093,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C8" s="4"/>
       <c r="D8" s="9">
         <v>120</v>
@@ -1940,7 +2117,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="4"/>
       <c r="D9" s="12">
         <v>150</v>
@@ -1964,7 +2141,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1981,7 +2158,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1998,7 +2175,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2015,7 +2192,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2032,7 +2209,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2049,7 +2226,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2066,7 +2243,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2083,7 +2260,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2100,7 +2277,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2117,7 +2294,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2134,7 +2311,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2151,7 +2328,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2173,4 +2350,379 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:T17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25" style="3" customWidth="1"/>
+    <col min="6" max="9" width="22.7265625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C3" s="4"/>
+      <c r="D3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C4" s="4"/>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20">
+        <v>30.4</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="19">
+        <v>170</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="4"/>
+      <c r="D5" s="12">
+        <v>90</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18">
+        <v>15.2</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="17">
+        <v>88</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+      <c r="D9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="1"/>
+      <c r="D11" s="12">
+        <v>90</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added question 5.2i and 5.2j for lab2a
</commit_message>
<xml_diff>
--- a/lab2a/tabelas/tabelas comando conversor.xlsx
+++ b/lab2a/tabelas/tabelas comando conversor.xlsx
@@ -764,11 +764,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="249641184"/>
-        <c:axId val="249642752"/>
+        <c:axId val="257576000"/>
+        <c:axId val="257579136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="249641184"/>
+        <c:axId val="257576000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,7 +871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249642752"/>
+        <c:crossAx val="257579136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -879,7 +879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="249642752"/>
+        <c:axId val="257579136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,7 +985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249641184"/>
+        <c:crossAx val="257576000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2356,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2426,8 +2426,12 @@
       <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="20"/>
+      <c r="E4" s="10">
+        <v>191.8</v>
+      </c>
+      <c r="F4" s="20">
+        <v>44.54</v>
+      </c>
       <c r="G4" s="20">
         <v>30.4</v>
       </c>
@@ -2452,7 +2456,9 @@
       <c r="D5" s="12">
         <v>90</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13">
+        <v>101.82899999999999</v>
+      </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18">
         <v>15.2</v>
@@ -2562,7 +2568,9 @@
       <c r="D10" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="11">
+        <v>191.8</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -2584,7 +2592,9 @@
       <c r="D11" s="12">
         <v>90</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14">
+        <v>101.82899999999999</v>
+      </c>
       <c r="F11" s="8"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>

</xml_diff>